<commit_message>
ing update & 나승원 PSP 수정
</commit_message>
<xml_diff>
--- a/Project Documentation/1_3_PSP_Sheet.xlsx
+++ b/Project Documentation/1_3_PSP_Sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Programming\babalzza-master\babalzza-master\Project Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A359273-1E9B-4896-9989-2EB8246442CE}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB9274A6-1BE1-470F-B43F-0E428666245B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="384" yWindow="384" windowWidth="17280" windowHeight="10020" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="백지수" sheetId="1" r:id="rId1"/>
@@ -1125,7 +1125,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="653" uniqueCount="242">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="655" uniqueCount="244">
   <si>
     <r>
       <rPr>
@@ -12100,6 +12100,7 @@
         <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> </t>
     </r>
@@ -12118,6 +12119,7 @@
         <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> </t>
     </r>
@@ -12136,6 +12138,7 @@
         <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> </t>
     </r>
@@ -12168,6 +12171,26 @@
         <charset val="129"/>
       </rPr>
       <t>), Entity class 수정</t>
+    </r>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>기능 개발</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>테이블</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve"> 단일 데이터베이스 내 저장 및 Entity Class Refactoring</t>
     </r>
     <phoneticPr fontId="9" type="noConversion"/>
   </si>
@@ -15750,8 +15773,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:G62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="89" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G51" sqref="G51"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="89" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F52" sqref="F52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.2"/>
@@ -16967,17 +16990,29 @@
         <v>241</v>
       </c>
     </row>
-    <row r="54" spans="1:7">
-      <c r="A54" s="87"/>
-      <c r="B54" s="51"/>
-      <c r="C54" s="51"/>
-      <c r="D54" s="32"/>
+    <row r="54" spans="1:7" ht="13.8">
+      <c r="A54" s="114">
+        <v>43796</v>
+      </c>
+      <c r="B54" s="51">
+        <v>0.625</v>
+      </c>
+      <c r="C54" s="51">
+        <v>0.8125</v>
+      </c>
+      <c r="D54" s="32">
+        <v>10</v>
+      </c>
       <c r="E54" s="58">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F54" s="6"/>
-      <c r="G54" s="39"/>
+        <v>0.18055555555555555</v>
+      </c>
+      <c r="F54" s="115" t="s">
+        <v>242</v>
+      </c>
+      <c r="G54" s="113" t="s">
+        <v>243</v>
+      </c>
     </row>
     <row r="55" spans="1:7">
       <c r="A55" s="87"/>

</xml_diff>

<commit_message>
김정현 PSP 수정 & 식단추천 Activity 1128
</commit_message>
<xml_diff>
--- a/Project Documentation/1_3_PSP_Sheet.xlsx
+++ b/Project Documentation/1_3_PSP_Sheet.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Programming\babalzza-master\babalzza-master\Project Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kimjh\Desktop\babalzza-master\babalzza-master\Project Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85245168-425F-4551-B5CF-ED611A8DA1CB}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4F10DBA-8D70-45EA-ADC4-874EA972F504}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="8964" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="백지수" sheetId="1" r:id="rId1"/>
@@ -1125,7 +1125,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="674" uniqueCount="253">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="692" uniqueCount="263">
   <si>
     <r>
       <rPr>
@@ -11245,49 +11245,6 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Initial Data Set </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="돋움"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>수정</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> (</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="돋움"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>수량추가</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>)</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t>기능</t>
     </r>
     <r>
@@ -12546,6 +12503,303 @@
   </si>
   <si>
     <t>식재료 관리 데이터베이스 구축 code 및 UI 호환 code 통합</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Project Documentation </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>및</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Data Set </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>업데이트</t>
+    </r>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Project Documentation </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>및</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> Data Set </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>업데이트</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Initial Data Set </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>수정</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>수량추가</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>)</t>
+    </r>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Initial Data Set </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>수정</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>수량추가</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <t>기능 개발</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>식단</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>추천</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> Activity </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>개발</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>11</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>월</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> 24</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>일</t>
+    </r>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>11월 25</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>일</t>
+    </r>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>11월 26</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>일</t>
+    </r>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>11월 27</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>일</t>
+    </r>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>11월 28</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>일</t>
+    </r>
     <phoneticPr fontId="9" type="noConversion"/>
   </si>
 </sst>
@@ -13316,19 +13570,19 @@
       <selection activeCell="E87" sqref="E87"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="11.44140625" style="87" customWidth="1"/>
-    <col min="2" max="2" width="8.6640625" style="51" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" style="87" customWidth="1"/>
+    <col min="2" max="2" width="8.7109375" style="51" customWidth="1"/>
     <col min="3" max="3" width="7" style="51" customWidth="1"/>
-    <col min="4" max="4" width="11.44140625" style="32" customWidth="1"/>
-    <col min="5" max="5" width="11.44140625" style="58" customWidth="1"/>
-    <col min="6" max="6" width="25.6640625" style="19" customWidth="1"/>
-    <col min="7" max="7" width="46.44140625" style="39" customWidth="1"/>
-    <col min="14" max="14" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" style="32" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" style="58" customWidth="1"/>
+    <col min="6" max="6" width="25.7109375" style="19" customWidth="1"/>
+    <col min="7" max="7" width="46.42578125" style="39" customWidth="1"/>
+    <col min="14" max="14" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="11.7" customHeight="1">
+    <row r="1" spans="1:7" ht="11.65" customHeight="1">
       <c r="A1" s="96" t="s">
         <v>41</v>
       </c>
@@ -13341,10 +13595,10 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="11.7" customHeight="1">
+    <row r="2" spans="1:7" ht="11.65" customHeight="1">
       <c r="A2" s="89"/>
     </row>
-    <row r="3" spans="1:7" ht="11.7" customHeight="1">
+    <row r="3" spans="1:7" ht="11.65" customHeight="1">
       <c r="A3" s="97" t="s">
         <v>127</v>
       </c>
@@ -13355,8 +13609,8 @@
       <c r="E3" s="77"/>
       <c r="F3" s="39"/>
     </row>
-    <row r="4" spans="1:7" ht="11.7" customHeight="1"/>
-    <row r="5" spans="1:7" s="7" customFormat="1" ht="26.4">
+    <row r="4" spans="1:7" ht="11.65" customHeight="1"/>
+    <row r="5" spans="1:7" s="7" customFormat="1" ht="25.5">
       <c r="A5" s="98" t="s">
         <v>129</v>
       </c>
@@ -13571,7 +13825,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="13.8">
+    <row r="14" spans="1:7">
       <c r="A14" s="87">
         <v>43728</v>
       </c>
@@ -13691,7 +13945,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="13.8">
+    <row r="19" spans="1:7">
       <c r="A19" s="87">
         <v>43739</v>
       </c>
@@ -13787,7 +14041,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="13.8">
+    <row r="23" spans="1:7">
       <c r="A23" s="89">
         <v>43748</v>
       </c>
@@ -13811,7 +14065,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="13.8">
+    <row r="24" spans="1:7">
       <c r="A24" s="95">
         <v>43749</v>
       </c>
@@ -13859,7 +14113,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="13.8">
+    <row r="26" spans="1:7">
       <c r="A26" s="89">
         <v>43755</v>
       </c>
@@ -13883,7 +14137,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="13.8">
+    <row r="27" spans="1:7">
       <c r="A27" s="89">
         <v>43755</v>
       </c>
@@ -13907,7 +14161,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="13.8">
+    <row r="28" spans="1:7">
       <c r="A28" s="89">
         <v>43755</v>
       </c>
@@ -13931,7 +14185,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="13.8">
+    <row r="29" spans="1:7">
       <c r="A29" s="89">
         <v>43761</v>
       </c>
@@ -14195,7 +14449,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="40" spans="1:7" ht="14.7" customHeight="1">
+    <row r="40" spans="1:7" ht="14.65" customHeight="1">
       <c r="A40" s="95">
         <v>43767</v>
       </c>
@@ -14219,7 +14473,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="41" spans="1:7" ht="14.7" customHeight="1">
+    <row r="41" spans="1:7" ht="14.65" customHeight="1">
       <c r="A41" s="95">
         <v>43769</v>
       </c>
@@ -14339,7 +14593,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="46" spans="1:7" ht="13.8">
+    <row r="46" spans="1:7">
       <c r="A46" s="87">
         <v>43770</v>
       </c>
@@ -14363,7 +14617,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="47" spans="1:7" ht="13.8">
+    <row r="47" spans="1:7">
       <c r="A47" s="87">
         <v>43770</v>
       </c>
@@ -14387,7 +14641,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="48" spans="1:7" ht="13.8">
+    <row r="48" spans="1:7">
       <c r="A48" s="95" t="s">
         <v>138</v>
       </c>
@@ -14411,7 +14665,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="49" spans="1:7" ht="13.8">
+    <row r="49" spans="1:7">
       <c r="A49" s="99" t="s">
         <v>138</v>
       </c>
@@ -14435,7 +14689,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="50" spans="1:7" ht="13.8">
+    <row r="50" spans="1:7">
       <c r="A50" s="87">
         <v>43774</v>
       </c>
@@ -14459,7 +14713,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="51" spans="1:7" ht="13.8">
+    <row r="51" spans="1:7">
       <c r="A51" s="87">
         <v>43774</v>
       </c>
@@ -14483,7 +14737,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="52" spans="1:7" ht="13.8">
+    <row r="52" spans="1:7">
       <c r="A52" s="87">
         <v>43775</v>
       </c>
@@ -14507,7 +14761,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="53" spans="1:7" ht="13.8">
+    <row r="53" spans="1:7">
       <c r="A53" s="87">
         <v>43776</v>
       </c>
@@ -14531,7 +14785,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="54" spans="1:7" ht="13.8">
+    <row r="54" spans="1:7">
       <c r="A54" s="87">
         <v>43776</v>
       </c>
@@ -14555,7 +14809,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="55" spans="1:7" ht="13.8">
+    <row r="55" spans="1:7">
       <c r="A55" s="87">
         <v>43778</v>
       </c>
@@ -14579,7 +14833,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="56" spans="1:7" ht="13.8">
+    <row r="56" spans="1:7">
       <c r="A56" s="87">
         <v>43779</v>
       </c>
@@ -14603,7 +14857,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="57" spans="1:7" ht="13.8">
+    <row r="57" spans="1:7">
       <c r="A57" s="87">
         <v>43780</v>
       </c>
@@ -14627,7 +14881,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="58" spans="1:7" ht="13.8">
+    <row r="58" spans="1:7">
       <c r="A58" s="87">
         <v>43781</v>
       </c>
@@ -14651,7 +14905,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="59" spans="1:7" ht="13.8">
+    <row r="59" spans="1:7">
       <c r="A59" s="87">
         <v>43781</v>
       </c>
@@ -14675,7 +14929,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="60" spans="1:7" ht="13.8">
+    <row r="60" spans="1:7">
       <c r="A60" s="87">
         <v>43781</v>
       </c>
@@ -14699,7 +14953,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="61" spans="1:7" ht="13.8">
+    <row r="61" spans="1:7">
       <c r="A61" s="87">
         <v>43782</v>
       </c>
@@ -14723,7 +14977,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="62" spans="1:7" ht="13.8">
+    <row r="62" spans="1:7">
       <c r="A62" s="87">
         <v>43782</v>
       </c>
@@ -14747,7 +15001,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="63" spans="1:7" ht="13.8">
+    <row r="63" spans="1:7">
       <c r="A63" s="87">
         <v>43785</v>
       </c>
@@ -14771,7 +15025,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="64" spans="1:7" ht="13.8">
+    <row r="64" spans="1:7">
       <c r="A64" s="87">
         <v>43785</v>
       </c>
@@ -14792,10 +15046,10 @@
         <v>186</v>
       </c>
       <c r="G64" s="113" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="65" spans="1:14" ht="13.8">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="65" spans="1:14">
       <c r="A65" s="87">
         <v>43785</v>
       </c>
@@ -14816,10 +15070,10 @@
         <v>186</v>
       </c>
       <c r="G65" s="113" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="66" spans="1:14" ht="13.8">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="66" spans="1:14">
       <c r="A66" s="87">
         <v>43786</v>
       </c>
@@ -14840,10 +15094,10 @@
         <v>186</v>
       </c>
       <c r="G66" s="113" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="67" spans="1:14" ht="13.8">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="67" spans="1:14">
       <c r="A67" s="87">
         <v>43788</v>
       </c>
@@ -14864,10 +15118,10 @@
         <v>186</v>
       </c>
       <c r="G67" s="113" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="68" spans="1:14" ht="13.8">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="68" spans="1:14">
       <c r="A68" s="87">
         <v>43791</v>
       </c>
@@ -14888,10 +15142,10 @@
         <v>186</v>
       </c>
       <c r="G68" s="113" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="69" spans="1:14" ht="13.8">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="69" spans="1:14">
       <c r="A69" s="87">
         <v>43791</v>
       </c>
@@ -14915,7 +15169,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="70" spans="1:14" ht="13.8">
+    <row r="70" spans="1:14">
       <c r="A70" s="87">
         <v>43792</v>
       </c>
@@ -14939,7 +15193,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="71" spans="1:14" ht="13.8">
+    <row r="71" spans="1:14">
       <c r="A71" s="87">
         <v>43792</v>
       </c>
@@ -14963,7 +15217,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="72" spans="1:14" ht="13.8">
+    <row r="72" spans="1:14">
       <c r="A72" s="87">
         <v>43793</v>
       </c>
@@ -14981,14 +15235,14 @@
         <v>6.25E-2</v>
       </c>
       <c r="F72" s="116" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="G72" s="113" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="N72" s="107"/>
     </row>
-    <row r="73" spans="1:14" ht="13.8">
+    <row r="73" spans="1:14">
       <c r="A73" s="87">
         <v>43793</v>
       </c>
@@ -15009,10 +15263,10 @@
         <v>186</v>
       </c>
       <c r="G73" s="113" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="74" spans="1:14" ht="13.8">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="74" spans="1:14">
       <c r="A74" s="87">
         <v>43793</v>
       </c>
@@ -15036,7 +15290,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="75" spans="1:14" ht="13.8">
+    <row r="75" spans="1:14">
       <c r="A75" s="87">
         <v>43793</v>
       </c>
@@ -15060,7 +15314,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="76" spans="1:14" ht="13.8">
+    <row r="76" spans="1:14">
       <c r="A76" s="87">
         <v>43794</v>
       </c>
@@ -15081,10 +15335,10 @@
         <v>186</v>
       </c>
       <c r="G76" s="39" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="77" spans="1:14" ht="13.8">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="77" spans="1:14">
       <c r="A77" s="87">
         <v>43794</v>
       </c>
@@ -15105,10 +15359,10 @@
         <v>186</v>
       </c>
       <c r="G77" s="39" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="78" spans="1:14" ht="13.8">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="78" spans="1:14">
       <c r="A78" s="87">
         <v>43794</v>
       </c>
@@ -15129,10 +15383,10 @@
         <v>186</v>
       </c>
       <c r="G78" s="39" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="79" spans="1:14" ht="13.8">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="79" spans="1:14">
       <c r="A79" s="87">
         <v>43795</v>
       </c>
@@ -15150,13 +15404,13 @@
         <v>0.2013888888888889</v>
       </c>
       <c r="F79" s="116" t="s">
+        <v>228</v>
+      </c>
+      <c r="G79" s="37" t="s">
         <v>229</v>
       </c>
-      <c r="G79" s="37" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="80" spans="1:14" ht="13.8">
+    </row>
+    <row r="80" spans="1:14">
       <c r="A80" s="87">
         <v>43795</v>
       </c>
@@ -15174,13 +15428,13 @@
         <v>4.166666666666663E-2</v>
       </c>
       <c r="F80" s="116" t="s">
+        <v>228</v>
+      </c>
+      <c r="G80" s="37" t="s">
         <v>229</v>
       </c>
-      <c r="G80" s="37" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="81" spans="1:7" ht="13.8">
+    </row>
+    <row r="81" spans="1:7">
       <c r="A81" s="87">
         <v>43795</v>
       </c>
@@ -15198,13 +15452,13 @@
         <v>2.777777777777779E-2</v>
       </c>
       <c r="F81" s="116" t="s">
+        <v>230</v>
+      </c>
+      <c r="G81" s="113" t="s">
         <v>231</v>
       </c>
-      <c r="G81" s="113" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="82" spans="1:7" ht="13.8">
+    </row>
+    <row r="82" spans="1:7">
       <c r="A82" s="87">
         <v>43795</v>
       </c>
@@ -15225,10 +15479,10 @@
         <v>186</v>
       </c>
       <c r="G82" s="113" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="83" spans="1:7" ht="13.8">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7">
       <c r="A83" s="87">
         <v>43795</v>
       </c>
@@ -15249,10 +15503,10 @@
         <v>186</v>
       </c>
       <c r="G83" s="113" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="84" spans="1:7" ht="13.8">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7">
       <c r="A84" s="87">
         <v>43796</v>
       </c>
@@ -15273,10 +15527,10 @@
         <v>186</v>
       </c>
       <c r="G84" s="113" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="85" spans="1:7" ht="13.8">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7">
       <c r="A85" s="87">
         <v>43796</v>
       </c>
@@ -15294,13 +15548,13 @@
         <v>0.14583333333333329</v>
       </c>
       <c r="F85" s="116" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="G85" s="113" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="86" spans="1:7" ht="13.8">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7">
       <c r="A86" s="87">
         <v>43796</v>
       </c>
@@ -15318,10 +15572,10 @@
         <v>0.17361111111111119</v>
       </c>
       <c r="F86" s="116" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="G86" s="39" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
   </sheetData>
@@ -15340,21 +15594,21 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:N45"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScale="77" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="G36" sqref="G36"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="E45" sqref="E45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="10" style="85" customWidth="1"/>
     <col min="2" max="3" width="7" style="53" customWidth="1"/>
-    <col min="4" max="4" width="11.44140625" style="60" customWidth="1"/>
-    <col min="5" max="5" width="9.6640625" style="5" customWidth="1"/>
-    <col min="6" max="6" width="25.44140625" style="5" customWidth="1"/>
-    <col min="7" max="7" width="55.44140625" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" style="60" customWidth="1"/>
+    <col min="5" max="5" width="9.7109375" style="5" customWidth="1"/>
+    <col min="6" max="6" width="25.42578125" style="5" customWidth="1"/>
+    <col min="7" max="7" width="55.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="11.7" customHeight="1">
+    <row r="1" spans="1:10" ht="11.65" customHeight="1">
       <c r="A1" s="9" t="s">
         <v>41</v>
       </c>
@@ -15367,10 +15621,10 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="11.7" customHeight="1">
+    <row r="2" spans="1:10" ht="11.65" customHeight="1">
       <c r="A2" s="92"/>
     </row>
-    <row r="3" spans="1:10" ht="11.7" customHeight="1">
+    <row r="3" spans="1:10" ht="11.65" customHeight="1">
       <c r="A3" s="93" t="s">
         <v>127</v>
       </c>
@@ -15381,8 +15635,8 @@
       <c r="E3"/>
       <c r="F3"/>
     </row>
-    <row r="4" spans="1:10" ht="11.7" customHeight="1"/>
-    <row r="5" spans="1:10" s="7" customFormat="1" ht="26.4">
+    <row r="4" spans="1:10" ht="11.65" customHeight="1"/>
+    <row r="5" spans="1:10" s="7" customFormat="1" ht="25.5">
       <c r="A5" s="86" t="s">
         <v>129</v>
       </c>
@@ -15598,7 +15852,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="15.6">
+    <row r="14" spans="1:10" ht="13.5">
       <c r="A14" s="89" t="s">
         <v>131</v>
       </c>
@@ -15622,7 +15876,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="15.6">
+    <row r="15" spans="1:10" ht="13.5">
       <c r="A15" s="89">
         <v>43746</v>
       </c>
@@ -15646,7 +15900,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="15.6">
+    <row r="16" spans="1:10" ht="13.5">
       <c r="A16" s="89">
         <v>43748</v>
       </c>
@@ -15670,7 +15924,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="15.6">
+    <row r="17" spans="1:7" ht="13.5">
       <c r="A17" s="87">
         <v>43749</v>
       </c>
@@ -15694,7 +15948,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="13.8">
+    <row r="18" spans="1:7">
       <c r="A18" s="50">
         <v>43749</v>
       </c>
@@ -15718,7 +15972,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="13.8">
+    <row r="19" spans="1:7">
       <c r="A19" s="47">
         <v>43755</v>
       </c>
@@ -15742,7 +15996,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="13.8">
+    <row r="20" spans="1:7">
       <c r="A20" s="47">
         <v>43755</v>
       </c>
@@ -15862,7 +16116,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="14.7" customHeight="1">
+    <row r="25" spans="1:7" ht="14.65" customHeight="1">
       <c r="A25" s="50">
         <v>43769</v>
       </c>
@@ -15910,7 +16164,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="15.6">
+    <row r="27" spans="1:7" ht="13.5">
       <c r="A27" s="99" t="s">
         <v>145</v>
       </c>
@@ -15934,7 +16188,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="13.8">
+    <row r="28" spans="1:7">
       <c r="A28" s="87">
         <v>43779</v>
       </c>
@@ -15958,7 +16212,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="13.8">
+    <row r="29" spans="1:7">
       <c r="A29" s="87">
         <v>43782</v>
       </c>
@@ -15982,7 +16236,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="15.6">
+    <row r="30" spans="1:7" ht="13.5">
       <c r="A30" s="114" t="s">
         <v>181</v>
       </c>
@@ -16028,7 +16282,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="15.6">
+    <row r="32" spans="1:7" ht="13.5">
       <c r="A32" s="114" t="s">
         <v>205</v>
       </c>
@@ -16051,7 +16305,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="33" spans="1:14" ht="15.6">
+    <row r="33" spans="1:14" ht="13.5">
       <c r="A33" s="114" t="s">
         <v>207</v>
       </c>
@@ -16113,14 +16367,14 @@
       <c r="E35" s="13">
         <v>180</v>
       </c>
-      <c r="F35" s="13" t="s">
-        <v>203</v>
-      </c>
-      <c r="G35" s="2" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="36" spans="1:14" ht="13.8">
+      <c r="F35" s="112" t="s">
+        <v>252</v>
+      </c>
+      <c r="G35" s="113" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14">
       <c r="A36" s="87">
         <v>43793</v>
       </c>
@@ -16138,66 +16392,150 @@
         <v>4.166666666666663E-2</v>
       </c>
       <c r="F36" s="116" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="G36" s="113" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="N36" s="107"/>
     </row>
     <row r="37" spans="1:14" ht="15" customHeight="1">
-      <c r="A37" s="87"/>
-      <c r="B37" s="51"/>
-      <c r="C37" s="51"/>
-      <c r="D37" s="32"/>
-      <c r="E37" s="13"/>
-      <c r="F37" s="13"/>
-      <c r="G37" s="2"/>
+      <c r="A37" s="114" t="s">
+        <v>258</v>
+      </c>
+      <c r="B37" s="51">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="C37" s="51">
+        <v>0.77083333333333337</v>
+      </c>
+      <c r="D37" s="32">
+        <v>0</v>
+      </c>
+      <c r="E37" s="13">
+        <v>240</v>
+      </c>
+      <c r="F37" s="13" t="s">
+        <v>253</v>
+      </c>
+      <c r="G37" s="2" t="s">
+        <v>255</v>
+      </c>
     </row>
     <row r="38" spans="1:14" ht="15" customHeight="1">
-      <c r="A38" s="87"/>
-      <c r="B38" s="51"/>
-      <c r="C38" s="51"/>
-      <c r="D38" s="32"/>
-      <c r="E38" s="13"/>
-      <c r="F38" s="13"/>
-      <c r="G38" s="2"/>
+      <c r="A38" s="114" t="s">
+        <v>259</v>
+      </c>
+      <c r="B38" s="51">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="C38" s="51">
+        <v>0.9375</v>
+      </c>
+      <c r="D38" s="32">
+        <v>20</v>
+      </c>
+      <c r="E38" s="13">
+        <v>130</v>
+      </c>
+      <c r="F38" s="117" t="s">
+        <v>256</v>
+      </c>
+      <c r="G38" s="37" t="s">
+        <v>257</v>
+      </c>
     </row>
     <row r="39" spans="1:14" ht="15" customHeight="1">
-      <c r="A39" s="87"/>
-      <c r="B39" s="51"/>
-      <c r="C39" s="51"/>
-      <c r="D39" s="32"/>
-      <c r="E39" s="13"/>
-      <c r="F39" s="13"/>
-      <c r="G39" s="2"/>
+      <c r="A39" s="114" t="s">
+        <v>260</v>
+      </c>
+      <c r="B39" s="51">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="C39" s="51">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="D39" s="32">
+        <v>60</v>
+      </c>
+      <c r="E39" s="13">
+        <v>180</v>
+      </c>
+      <c r="F39" s="117" t="s">
+        <v>256</v>
+      </c>
+      <c r="G39" s="37" t="s">
+        <v>257</v>
+      </c>
     </row>
     <row r="40" spans="1:14" ht="15" customHeight="1">
-      <c r="A40" s="87"/>
-      <c r="B40" s="51"/>
-      <c r="C40" s="51"/>
-      <c r="D40" s="32"/>
-      <c r="E40" s="13"/>
-      <c r="F40" s="13"/>
-      <c r="G40" s="2"/>
+      <c r="A40" s="114" t="s">
+        <v>261</v>
+      </c>
+      <c r="B40" s="51">
+        <v>0.64583333333333337</v>
+      </c>
+      <c r="C40" s="51">
+        <v>0.77083333333333337</v>
+      </c>
+      <c r="D40" s="32">
+        <v>30</v>
+      </c>
+      <c r="E40" s="13">
+        <v>150</v>
+      </c>
+      <c r="F40" s="117" t="s">
+        <v>256</v>
+      </c>
+      <c r="G40" s="37" t="s">
+        <v>257</v>
+      </c>
     </row>
     <row r="41" spans="1:14" ht="15" customHeight="1">
-      <c r="A41" s="87"/>
-      <c r="B41" s="51"/>
-      <c r="C41" s="51"/>
-      <c r="D41" s="32"/>
-      <c r="E41" s="13"/>
-      <c r="F41" s="13"/>
-      <c r="G41" s="2"/>
+      <c r="A41" s="114" t="s">
+        <v>262</v>
+      </c>
+      <c r="B41" s="51">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="C41" s="51">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="D41" s="32">
+        <v>30</v>
+      </c>
+      <c r="E41" s="13">
+        <v>180</v>
+      </c>
+      <c r="F41" s="117" t="s">
+        <v>256</v>
+      </c>
+      <c r="G41" s="37" t="s">
+        <v>257</v>
+      </c>
     </row>
     <row r="42" spans="1:14" ht="15" customHeight="1">
-      <c r="A42" s="87"/>
-      <c r="B42" s="51"/>
-      <c r="C42" s="51"/>
-      <c r="D42" s="32"/>
-      <c r="E42" s="13"/>
-      <c r="F42" s="13"/>
-      <c r="G42" s="2"/>
+      <c r="A42" s="114" t="s">
+        <v>262</v>
+      </c>
+      <c r="B42" s="51">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="C42" s="51">
+        <v>0.55555555555555558</v>
+      </c>
+      <c r="D42" s="32">
+        <v>20</v>
+      </c>
+      <c r="E42" s="13">
+        <v>90</v>
+      </c>
+      <c r="F42" s="117" t="s">
+        <v>256</v>
+      </c>
+      <c r="G42" s="37" t="s">
+        <v>257</v>
+      </c>
     </row>
     <row r="43" spans="1:14" ht="15" customHeight="1">
       <c r="A43" s="87"/>
@@ -16242,21 +16580,21 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:G62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="89" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView topLeftCell="A31" zoomScale="89" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="G60" sqref="G60"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="10" customWidth="1"/>
     <col min="2" max="3" width="7" style="53" customWidth="1"/>
-    <col min="4" max="4" width="11.44140625" style="60" customWidth="1"/>
-    <col min="5" max="5" width="9.6640625" style="65" customWidth="1"/>
-    <col min="6" max="6" width="29.6640625" style="5" customWidth="1"/>
-    <col min="7" max="7" width="61.33203125" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" style="60" customWidth="1"/>
+    <col min="5" max="5" width="9.7109375" style="65" customWidth="1"/>
+    <col min="6" max="6" width="29.7109375" style="5" customWidth="1"/>
+    <col min="7" max="7" width="61.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="11.7" customHeight="1">
+    <row r="1" spans="1:7" ht="11.65" customHeight="1">
       <c r="A1" s="9" t="s">
         <v>41</v>
       </c>
@@ -16269,10 +16607,10 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="11.7" customHeight="1">
+    <row r="2" spans="1:7" ht="11.65" customHeight="1">
       <c r="A2" s="17"/>
     </row>
-    <row r="3" spans="1:7" ht="11.7" customHeight="1">
+    <row r="3" spans="1:7" ht="11.65" customHeight="1">
       <c r="A3" s="16" t="s">
         <v>127</v>
       </c>
@@ -16283,8 +16621,8 @@
       <c r="E3" s="66"/>
       <c r="F3"/>
     </row>
-    <row r="4" spans="1:7" ht="11.7" customHeight="1"/>
-    <row r="5" spans="1:7" s="7" customFormat="1" ht="26.4">
+    <row r="4" spans="1:7" ht="11.65" customHeight="1"/>
+    <row r="5" spans="1:7" s="7" customFormat="1" ht="25.5">
       <c r="A5" s="8" t="s">
         <v>129</v>
       </c>
@@ -16499,7 +16837,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="13.8">
+    <row r="14" spans="1:7">
       <c r="A14" s="10">
         <v>43739</v>
       </c>
@@ -16523,7 +16861,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="13.8">
+    <row r="15" spans="1:7">
       <c r="A15" s="35">
         <v>43739</v>
       </c>
@@ -16619,7 +16957,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="15.6">
+    <row r="19" spans="1:7" ht="13.5">
       <c r="A19" s="89">
         <v>43746</v>
       </c>
@@ -16643,7 +16981,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="15.6">
+    <row r="20" spans="1:7" ht="13.5">
       <c r="A20" s="89">
         <v>43748</v>
       </c>
@@ -16667,7 +17005,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="15.6">
+    <row r="21" spans="1:7" ht="13.5">
       <c r="A21" s="87">
         <v>43749</v>
       </c>
@@ -16691,7 +17029,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="13.8">
+    <row r="22" spans="1:7">
       <c r="A22" s="50">
         <v>43749</v>
       </c>
@@ -16715,7 +17053,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="15.6">
+    <row r="23" spans="1:7" ht="13.5">
       <c r="A23" s="35">
         <v>43750</v>
       </c>
@@ -16811,7 +17149,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="13.8">
+    <row r="27" spans="1:7">
       <c r="A27" s="47">
         <v>43755</v>
       </c>
@@ -16835,7 +17173,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="13.8">
+    <row r="28" spans="1:7">
       <c r="A28" s="47">
         <v>43755</v>
       </c>
@@ -16859,7 +17197,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="13.8">
+    <row r="29" spans="1:7">
       <c r="A29" s="10">
         <v>43760</v>
       </c>
@@ -16979,7 +17317,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="13.8">
+    <row r="34" spans="1:7">
       <c r="A34" s="35">
         <v>43770</v>
       </c>
@@ -17171,7 +17509,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="42" spans="1:7" ht="13.8">
+    <row r="42" spans="1:7">
       <c r="A42" s="87">
         <v>43779</v>
       </c>
@@ -17219,7 +17557,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="44" spans="1:7" ht="13.8">
+    <row r="44" spans="1:7">
       <c r="A44" s="87">
         <v>43782</v>
       </c>
@@ -17267,7 +17605,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="46" spans="1:7" ht="15.6">
+    <row r="46" spans="1:7" ht="13.5">
       <c r="A46" s="87">
         <v>43792</v>
       </c>
@@ -17285,13 +17623,13 @@
         <v>0.12499999999999997</v>
       </c>
       <c r="F46" s="121" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="G46" s="113" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" ht="13.8">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7">
       <c r="A47" s="87">
         <v>43793</v>
       </c>
@@ -17309,13 +17647,13 @@
         <v>4.166666666666663E-2</v>
       </c>
       <c r="F47" s="120" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="G47" s="113" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" ht="13.8">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7">
       <c r="A48" s="87">
         <v>43793</v>
       </c>
@@ -17333,13 +17671,13 @@
         <v>0.15277777777777785</v>
       </c>
       <c r="F48" s="120" t="s">
+        <v>215</v>
+      </c>
+      <c r="G48" s="113" t="s">
         <v>216</v>
       </c>
-      <c r="G48" s="113" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" ht="13.8">
+    </row>
+    <row r="49" spans="1:7">
       <c r="A49" s="87">
         <v>43794</v>
       </c>
@@ -17357,13 +17695,13 @@
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="F49" s="115" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="G49" s="113" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" ht="13.8">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7">
       <c r="A50" s="87">
         <v>43794</v>
       </c>
@@ -17381,13 +17719,13 @@
         <v>9.0277777777777873E-2</v>
       </c>
       <c r="F50" s="115" t="s">
+        <v>220</v>
+      </c>
+      <c r="G50" s="113" t="s">
         <v>221</v>
       </c>
-      <c r="G50" s="113" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" ht="13.8">
+    </row>
+    <row r="51" spans="1:7">
       <c r="A51" s="87">
         <v>43795</v>
       </c>
@@ -17405,13 +17743,13 @@
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="F51" s="120" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="G51" s="113" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" ht="13.8">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7">
       <c r="A52" s="87">
         <v>43795</v>
       </c>
@@ -17429,13 +17767,13 @@
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="F52" s="115" t="s">
+        <v>234</v>
+      </c>
+      <c r="G52" s="113" t="s">
         <v>235</v>
       </c>
-      <c r="G52" s="113" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" ht="13.8">
+    </row>
+    <row r="53" spans="1:7">
       <c r="A53" s="87">
         <v>43795</v>
       </c>
@@ -17453,13 +17791,13 @@
         <v>0.14583333333333334</v>
       </c>
       <c r="F53" s="120" t="s">
+        <v>236</v>
+      </c>
+      <c r="G53" s="113" t="s">
         <v>237</v>
       </c>
-      <c r="G53" s="113" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" ht="13.8">
+    </row>
+    <row r="54" spans="1:7">
       <c r="A54" s="114">
         <v>43796</v>
       </c>
@@ -17477,13 +17815,13 @@
         <v>0.18055555555555555</v>
       </c>
       <c r="F54" s="115" t="s">
+        <v>238</v>
+      </c>
+      <c r="G54" s="113" t="s">
         <v>239</v>
       </c>
-      <c r="G54" s="113" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" ht="13.8">
+    </row>
+    <row r="55" spans="1:7">
       <c r="A55" s="87">
         <v>43797</v>
       </c>
@@ -17501,13 +17839,13 @@
         <v>0.16666666666666666</v>
       </c>
       <c r="F55" s="115" t="s">
+        <v>249</v>
+      </c>
+      <c r="G55" s="37" t="s">
         <v>250</v>
       </c>
-      <c r="G55" s="37" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7" ht="13.8">
+    </row>
+    <row r="56" spans="1:7">
       <c r="A56" s="87">
         <v>43797</v>
       </c>
@@ -17525,10 +17863,10 @@
         <v>0.10416666666666669</v>
       </c>
       <c r="F56" s="120" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="G56" s="37" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="57" spans="1:7">
@@ -17623,17 +17961,17 @@
       <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="10" style="85" customWidth="1"/>
     <col min="2" max="3" width="7" style="53" customWidth="1"/>
-    <col min="4" max="4" width="11.44140625" style="60" customWidth="1"/>
-    <col min="5" max="5" width="9.44140625" style="65" customWidth="1"/>
-    <col min="6" max="6" width="16.6640625" style="5" customWidth="1"/>
-    <col min="7" max="7" width="46.44140625" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" style="60" customWidth="1"/>
+    <col min="5" max="5" width="9.42578125" style="65" customWidth="1"/>
+    <col min="6" max="6" width="16.7109375" style="5" customWidth="1"/>
+    <col min="7" max="7" width="46.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="11.7" customHeight="1">
+    <row r="1" spans="1:7" ht="11.65" customHeight="1">
       <c r="A1" s="9" t="s">
         <v>41</v>
       </c>
@@ -17646,10 +17984,10 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="11.7" customHeight="1">
+    <row r="2" spans="1:7" ht="11.65" customHeight="1">
       <c r="A2" s="92"/>
     </row>
-    <row r="3" spans="1:7" ht="11.7" customHeight="1">
+    <row r="3" spans="1:7" ht="11.65" customHeight="1">
       <c r="A3" s="93" t="s">
         <v>127</v>
       </c>
@@ -17660,8 +17998,8 @@
       <c r="E3" s="66"/>
       <c r="F3"/>
     </row>
-    <row r="4" spans="1:7" ht="11.7" customHeight="1"/>
-    <row r="5" spans="1:7" s="7" customFormat="1" ht="26.4">
+    <row r="4" spans="1:7" ht="11.65" customHeight="1"/>
+    <row r="5" spans="1:7" s="7" customFormat="1" ht="25.5">
       <c r="A5" s="86" t="s">
         <v>129</v>
       </c>
@@ -17828,7 +18166,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="15.6">
+    <row r="12" spans="1:7" ht="13.5">
       <c r="A12" s="89">
         <v>43746</v>
       </c>
@@ -17852,7 +18190,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="15.6">
+    <row r="13" spans="1:7" ht="13.5">
       <c r="A13" s="89">
         <v>43748</v>
       </c>
@@ -17876,7 +18214,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="15.6">
+    <row r="14" spans="1:7" ht="13.5">
       <c r="A14" s="87">
         <v>43749</v>
       </c>
@@ -17900,7 +18238,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="13.8">
+    <row r="15" spans="1:7">
       <c r="A15" s="50">
         <v>43749</v>
       </c>
@@ -17948,7 +18286,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="13.8">
+    <row r="17" spans="1:7">
       <c r="A17" s="47">
         <v>43755</v>
       </c>
@@ -18020,7 +18358,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="15.6">
+    <row r="20" spans="1:7" ht="13.5">
       <c r="A20" s="94" t="s">
         <v>141</v>
       </c>
@@ -18116,7 +18454,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="14.7" customHeight="1">
+    <row r="24" spans="1:7" ht="14.65" customHeight="1">
       <c r="A24" s="50">
         <v>43769</v>
       </c>
@@ -18164,7 +18502,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="13.8">
+    <row r="26" spans="1:7">
       <c r="A26" s="35">
         <v>43770</v>
       </c>
@@ -18188,7 +18526,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="13.8">
+    <row r="27" spans="1:7">
       <c r="A27" s="87">
         <v>43779</v>
       </c>
@@ -18212,7 +18550,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="13.8">
+    <row r="28" spans="1:7">
       <c r="A28" s="87">
         <v>43793</v>
       </c>
@@ -18233,10 +18571,10 @@
         <v>192</v>
       </c>
       <c r="G28" s="113" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" ht="13.8">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
       <c r="A29" s="87">
         <v>43794</v>
       </c>
@@ -18254,10 +18592,10 @@
         <v>0.13194444444444439</v>
       </c>
       <c r="F29" s="116" t="s">
+        <v>232</v>
+      </c>
+      <c r="G29" s="37" t="s">
         <v>233</v>
-      </c>
-      <c r="G29" s="37" t="s">
-        <v>234</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="15" customHeight="1">
@@ -18411,21 +18749,21 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:G101"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="85" zoomScaleNormal="106" workbookViewId="0">
+    <sheetView topLeftCell="A14" zoomScale="85" zoomScaleNormal="106" workbookViewId="0">
       <selection activeCell="A58" sqref="A58"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="16.33203125" style="85" customWidth="1"/>
+    <col min="1" max="1" width="16.28515625" style="85" customWidth="1"/>
     <col min="2" max="3" width="7" style="53" customWidth="1"/>
-    <col min="4" max="4" width="11.44140625" style="60" customWidth="1"/>
-    <col min="5" max="5" width="9.6640625" style="65" customWidth="1"/>
-    <col min="6" max="6" width="38.33203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" style="60" customWidth="1"/>
+    <col min="5" max="5" width="9.7109375" style="65" customWidth="1"/>
+    <col min="6" max="6" width="38.28515625" style="5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="62" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="11.7" customHeight="1">
+    <row r="1" spans="1:7" ht="11.65" customHeight="1">
       <c r="A1" s="9" t="s">
         <v>41</v>
       </c>
@@ -18438,10 +18776,10 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="11.7" customHeight="1">
+    <row r="2" spans="1:7" ht="11.65" customHeight="1">
       <c r="A2" s="83"/>
     </row>
-    <row r="3" spans="1:7" ht="11.7" customHeight="1">
+    <row r="3" spans="1:7" ht="11.65" customHeight="1">
       <c r="A3" s="84" t="s">
         <v>127</v>
       </c>
@@ -18452,8 +18790,8 @@
       <c r="E3" s="66"/>
       <c r="F3"/>
     </row>
-    <row r="4" spans="1:7" ht="11.7" customHeight="1"/>
-    <row r="5" spans="1:7" s="7" customFormat="1" ht="26.4">
+    <row r="4" spans="1:7" ht="11.65" customHeight="1"/>
+    <row r="5" spans="1:7" s="7" customFormat="1" ht="25.5">
       <c r="A5" s="86" t="s">
         <v>129</v>
       </c>
@@ -18476,7 +18814,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="13.8">
+    <row r="6" spans="1:7">
       <c r="A6" s="87">
         <v>43715</v>
       </c>
@@ -18500,7 +18838,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="13.8">
+    <row r="7" spans="1:7">
       <c r="A7" s="88">
         <v>43727</v>
       </c>
@@ -18524,7 +18862,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="13.8">
+    <row r="8" spans="1:7">
       <c r="A8" s="87">
         <v>43727</v>
       </c>
@@ -18548,7 +18886,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="13.8">
+    <row r="9" spans="1:7">
       <c r="A9" s="87">
         <v>43728</v>
       </c>
@@ -18596,7 +18934,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="13.8">
+    <row r="11" spans="1:7">
       <c r="A11" s="87">
         <v>43735</v>
       </c>
@@ -18620,7 +18958,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="13.8">
+    <row r="12" spans="1:7">
       <c r="A12" s="87">
         <v>43737</v>
       </c>
@@ -18644,7 +18982,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="13.8">
+    <row r="13" spans="1:7">
       <c r="A13" s="87">
         <v>43738</v>
       </c>
@@ -18668,7 +19006,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="13.8">
+    <row r="14" spans="1:7">
       <c r="A14" s="87">
         <v>43739</v>
       </c>
@@ -18692,7 +19030,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="13.8">
+    <row r="15" spans="1:7">
       <c r="A15" s="89">
         <v>43739</v>
       </c>
@@ -18716,7 +19054,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="13.8">
+    <row r="16" spans="1:7">
       <c r="A16" s="87">
         <v>43744</v>
       </c>
@@ -18740,7 +19078,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="13.8">
+    <row r="17" spans="1:7">
       <c r="A17" s="87">
         <v>43744</v>
       </c>
@@ -18764,7 +19102,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="13.8">
+    <row r="18" spans="1:7">
       <c r="A18" s="87">
         <v>43744</v>
       </c>
@@ -18788,7 +19126,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="15.6">
+    <row r="19" spans="1:7" ht="13.5">
       <c r="A19" s="89">
         <v>43746</v>
       </c>
@@ -18812,7 +19150,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="15.6">
+    <row r="20" spans="1:7" ht="13.5">
       <c r="A20" s="89">
         <v>43748</v>
       </c>
@@ -18836,7 +19174,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="15.6">
+    <row r="21" spans="1:7" ht="13.5">
       <c r="A21" s="87">
         <v>43749</v>
       </c>
@@ -18860,7 +19198,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="13.8">
+    <row r="22" spans="1:7">
       <c r="A22" s="50">
         <v>43749</v>
       </c>
@@ -18884,7 +19222,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="13.8">
+    <row r="23" spans="1:7">
       <c r="A23" s="87">
         <v>43751</v>
       </c>
@@ -18908,7 +19246,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="15.6">
+    <row r="24" spans="1:7" ht="13.5">
       <c r="A24" s="87">
         <v>43751</v>
       </c>
@@ -18980,7 +19318,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="13.8">
+    <row r="27" spans="1:7">
       <c r="A27" s="87">
         <v>43753</v>
       </c>
@@ -19028,7 +19366,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="13.8">
+    <row r="29" spans="1:7">
       <c r="A29" s="90">
         <v>43754</v>
       </c>
@@ -19052,7 +19390,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="13.8">
+    <row r="30" spans="1:7">
       <c r="A30" s="90">
         <v>43754</v>
       </c>
@@ -19100,7 +19438,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="13.8">
+    <row r="32" spans="1:7">
       <c r="A32" s="47">
         <v>43755</v>
       </c>
@@ -19124,7 +19462,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="14.7" customHeight="1">
+    <row r="33" spans="1:7" ht="14.65" customHeight="1">
       <c r="A33" s="90">
         <v>43755</v>
       </c>
@@ -19148,7 +19486,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="13.8">
+    <row r="34" spans="1:7">
       <c r="A34" s="47">
         <v>43755</v>
       </c>
@@ -19388,7 +19726,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="44" spans="1:7" ht="13.8">
+    <row r="44" spans="1:7">
       <c r="A44" s="35">
         <v>43770</v>
       </c>
@@ -19436,7 +19774,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="46" spans="1:7" ht="13.8">
+    <row r="46" spans="1:7">
       <c r="A46" s="35">
         <v>43772</v>
       </c>
@@ -19458,7 +19796,7 @@
       </c>
       <c r="G46" s="123"/>
     </row>
-    <row r="47" spans="1:7" ht="13.8">
+    <row r="47" spans="1:7">
       <c r="A47" s="87">
         <v>43779</v>
       </c>
@@ -19482,7 +19820,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="48" spans="1:7" ht="13.8">
+    <row r="48" spans="1:7">
       <c r="A48" s="87">
         <v>43782</v>
       </c>
@@ -19506,7 +19844,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="49" spans="1:7" ht="13.8">
+    <row r="49" spans="1:7">
       <c r="A49" s="35">
         <v>43783</v>
       </c>
@@ -19554,7 +19892,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="51" spans="1:7" ht="15.6">
+    <row r="51" spans="1:7" ht="13.5">
       <c r="A51" s="35">
         <v>43791</v>
       </c>
@@ -19578,7 +19916,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="52" spans="1:7" ht="15.6">
+    <row r="52" spans="1:7" ht="13.5">
       <c r="A52" s="35">
         <v>43792</v>
       </c>
@@ -19650,7 +19988,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="55" spans="1:7" ht="13.8">
+    <row r="55" spans="1:7">
       <c r="A55" s="87">
         <v>43793</v>
       </c>
@@ -19671,7 +20009,7 @@
         <v>192</v>
       </c>
       <c r="G55" s="113" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="56" spans="1:7">
@@ -19719,7 +20057,7 @@
         <v>192</v>
       </c>
       <c r="G57" s="113" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="58" spans="1:7">
@@ -20137,21 +20475,21 @@
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:G47"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" zoomScaleNormal="125" workbookViewId="0">
+    <sheetView topLeftCell="A26" zoomScaleNormal="125" workbookViewId="0">
       <selection activeCell="G43" sqref="G43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="10" style="85" customWidth="1"/>
     <col min="2" max="3" width="7" style="53" customWidth="1"/>
-    <col min="4" max="4" width="11.44140625" style="60" customWidth="1"/>
-    <col min="5" max="5" width="9.6640625" style="65" customWidth="1"/>
-    <col min="6" max="6" width="29.33203125" style="5" customWidth="1"/>
-    <col min="7" max="7" width="46.44140625" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" style="60" customWidth="1"/>
+    <col min="5" max="5" width="9.7109375" style="65" customWidth="1"/>
+    <col min="6" max="6" width="29.28515625" style="5" customWidth="1"/>
+    <col min="7" max="7" width="46.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="11.7" customHeight="1">
+    <row r="1" spans="1:7" ht="11.65" customHeight="1">
       <c r="A1" s="9" t="s">
         <v>41</v>
       </c>
@@ -20164,10 +20502,10 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="11.7" customHeight="1">
+    <row r="2" spans="1:7" ht="11.65" customHeight="1">
       <c r="A2" s="92"/>
     </row>
-    <row r="3" spans="1:7" ht="11.7" customHeight="1">
+    <row r="3" spans="1:7" ht="11.65" customHeight="1">
       <c r="A3" s="93" t="s">
         <v>127</v>
       </c>
@@ -20178,8 +20516,8 @@
       <c r="E3" s="66"/>
       <c r="F3"/>
     </row>
-    <row r="4" spans="1:7" ht="11.7" customHeight="1"/>
-    <row r="5" spans="1:7" s="7" customFormat="1" ht="26.4">
+    <row r="4" spans="1:7" ht="11.65" customHeight="1"/>
+    <row r="5" spans="1:7" s="7" customFormat="1" ht="25.5">
       <c r="A5" s="86" t="s">
         <v>129</v>
       </c>
@@ -20346,7 +20684,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="13.8">
+    <row r="12" spans="1:7">
       <c r="A12" s="87" t="s">
         <v>134</v>
       </c>
@@ -20418,7 +20756,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="15.6">
+    <row r="15" spans="1:7" ht="13.5">
       <c r="A15" s="89">
         <v>43746</v>
       </c>
@@ -20442,7 +20780,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="15.6">
+    <row r="16" spans="1:7" ht="13.5">
       <c r="A16" s="89">
         <v>43748</v>
       </c>
@@ -20466,7 +20804,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="15.6">
+    <row r="17" spans="1:7" ht="13.5">
       <c r="A17" s="87">
         <v>43749</v>
       </c>
@@ -20490,7 +20828,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="13.8">
+    <row r="18" spans="1:7">
       <c r="A18" s="95">
         <v>43749</v>
       </c>
@@ -20562,7 +20900,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="13.8">
+    <row r="21" spans="1:7">
       <c r="A21" s="47">
         <v>43755</v>
       </c>
@@ -20586,7 +20924,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="13.8">
+    <row r="22" spans="1:7">
       <c r="A22" s="47">
         <v>43755</v>
       </c>
@@ -20730,7 +21068,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="14.7" customHeight="1">
+    <row r="28" spans="1:7" ht="14.65" customHeight="1">
       <c r="A28" s="50">
         <v>43769</v>
       </c>
@@ -20848,7 +21186,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="13.8">
+    <row r="33" spans="1:7">
       <c r="A33" s="87">
         <v>43782</v>
       </c>
@@ -20872,7 +21210,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="13.8">
+    <row r="34" spans="1:7">
       <c r="A34" s="114" t="s">
         <v>190</v>
       </c>
@@ -20987,7 +21325,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="39" spans="1:7" ht="13.8">
+    <row r="39" spans="1:7">
       <c r="A39" s="87">
         <v>43793</v>
       </c>
@@ -21008,7 +21346,7 @@
         <v>192</v>
       </c>
       <c r="G39" s="113" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="40" spans="1:7" ht="15" customHeight="1">
@@ -21036,7 +21374,7 @@
     </row>
     <row r="41" spans="1:7" ht="15" customHeight="1">
       <c r="A41" s="114" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B41" s="51">
         <v>0.54166666666666663</v>
@@ -21059,7 +21397,7 @@
     </row>
     <row r="42" spans="1:7" ht="15" customHeight="1">
       <c r="A42" s="114" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B42" s="51">
         <v>0.75</v>
@@ -21082,7 +21420,7 @@
     </row>
     <row r="43" spans="1:7" ht="15" customHeight="1">
       <c r="A43" s="114" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B43" s="51">
         <v>0.79166666666666663</v>

</xml_diff>